<commit_message>
robust facility location completed
</commit_message>
<xml_diff>
--- a/RobustFacilityLocation/results/summary.xlsx
+++ b/RobustFacilityLocation/results/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagan024\Desktop\CCG-RODDU\RobustFacilityLocation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagan024\Desktop\CCG-RODDU\RobustFacilityLocation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898B2013-E310-4CCA-9365-20A5324AAE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1586CAF-3E34-40CD-B5CF-DCBFA74A96E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -36,27 +36,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>alpha</t>
   </si>
   <si>
-    <t>Average objective value</t>
-  </si>
-  <si>
     <t>Reformulation</t>
   </si>
   <si>
-    <t>CCG</t>
-  </si>
-  <si>
     <t>Average computation time (s)</t>
+  </si>
+  <si>
+    <t>Single cut PCP</t>
+  </si>
+  <si>
+    <t>Multi-cut PCP</t>
+  </si>
+  <si>
+    <t># iters</t>
+  </si>
+  <si>
+    <t># cuts</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>N/A (10)</t>
+  </si>
+  <si>
+    <t>8.4(5)</t>
   </si>
 </sst>
 </file>
@@ -64,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -103,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -112,6 +124,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,222 +408,548 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="13" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" dyDescent="0.25" s="1" customFormat="1">
-      <c r="A1" t="s" s="1">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s" s="4">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" dyDescent="0.25" s="1" customFormat="1">
-      <c r="E2" t="s" s="1">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="1">
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="1">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s" s="1">
+      <c r="C3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="K3" s="5">
+        <v>6.6</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="5">
+        <v>10</v>
+      </c>
+      <c r="O3" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
+      <c r="P3" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="R3" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="S3" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="T3" s="5">
+        <v>2</v>
+      </c>
+      <c r="U3" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="V3" s="5">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2</v>
+      </c>
+      <c r="J4" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="K4" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="5">
+        <v>10</v>
+      </c>
+      <c r="O4" s="5">
+        <v>10</v>
+      </c>
+      <c r="P4" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="R4" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="S4" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="T4" s="5">
+        <v>2</v>
+      </c>
+      <c r="U4" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="V4" s="5">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B5" s="5">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C5" s="5">
         <v>0.01</v>
       </c>
-      <c r="E3"/>
-      <c r="F3">
-        <v>52.60045981190815</v>
-      </c>
-      <c r="G3">
-        <v>1457.7424083709716</v>
-      </c>
-      <c r="H3">
-        <v>2.1235198590817754</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="J5" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="K5" s="5">
+        <v>14.7</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="5">
         <v>20</v>
       </c>
-      <c r="B4">
+      <c r="O5" s="5">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>0.02</v>
-      </c>
-      <c r="E4"/>
-      <c r="F4">
-        <v>52.60045981190844</v>
-      </c>
-      <c r="G4">
-        <v>2304.405610370636</v>
-      </c>
-      <c r="H4">
-        <v>1.9389472537586303</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
+      <c r="P5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="R5" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="S5" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="T5" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="U5" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="V5" s="5">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5.9</v>
+      </c>
+      <c r="G6" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>4.7</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="K6" s="5">
+        <v>24.8</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="5">
+        <v>30</v>
+      </c>
+      <c r="O6" s="5">
+        <v>15</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>5.9</v>
+      </c>
+      <c r="R6" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="S6" s="5">
+        <v>4.7</v>
+      </c>
+      <c r="T6" s="5">
+        <v>2</v>
+      </c>
+      <c r="U6" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="V6" s="5">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>40</v>
       </c>
-      <c r="B5">
+      <c r="B7" s="5">
         <v>15</v>
       </c>
-      <c r="C5">
+      <c r="C7" s="5">
         <v>0.01</v>
       </c>
-      <c r="E5">
-        <v>279.15458778466785</v>
-      </c>
-      <c r="F5">
-        <v>275.249509090116</v>
-      </c>
-      <c r="G5">
-        <v>3600.9433101892473</v>
-      </c>
-      <c r="H5">
-        <v>6.970353797747277</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2</v>
+      </c>
+      <c r="J7" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="K7" s="5">
+        <v>34.1</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="5">
         <v>40</v>
       </c>
-      <c r="B6">
+      <c r="O7" s="5">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>0.02</v>
-      </c>
-      <c r="E6">
-        <v>275.24949296057514</v>
-      </c>
-      <c r="F6">
-        <v>275.24950909011613</v>
-      </c>
-      <c r="G6">
-        <v>3601.090216231346</v>
-      </c>
-      <c r="H6">
-        <v>6.691183625458068</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
+      <c r="P7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="R7" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="S7" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="T7" s="5">
+        <v>2</v>
+      </c>
+      <c r="U7" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="V7" s="5">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>40</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="5">
         <v>25</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="5">
         <v>0.01</v>
       </c>
-      <c r="E7">
-        <v>189.96002532681896</v>
-      </c>
-      <c r="F7">
-        <v>189.63520378646012</v>
-      </c>
-      <c r="G7">
-        <v>3603.518489289284</v>
-      </c>
-      <c r="H7">
-        <v>6.186067586035035</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>11.4</v>
+      </c>
+      <c r="H8" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="I8" s="5">
+        <v>2</v>
+      </c>
+      <c r="J8" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="K8" s="5">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="5">
         <v>40</v>
       </c>
-      <c r="B8">
+      <c r="O8" s="5">
         <v>25</v>
       </c>
-      <c r="C8">
-        <v>0.02</v>
-      </c>
-      <c r="E8">
-        <v>195.17481352826925</v>
-      </c>
-      <c r="F8">
-        <v>189.6352032832054</v>
-      </c>
-      <c r="G8">
-        <v>3602.3401066541674</v>
-      </c>
-      <c r="H8">
-        <v>7.097437890992163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>80</v>
-      </c>
-      <c r="B9">
-        <v>35</v>
-      </c>
-      <c r="C9">
+      <c r="P8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="R8" s="5">
+        <v>11.4</v>
+      </c>
+      <c r="S8" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="T8" s="5">
+        <v>2</v>
+      </c>
+      <c r="U8" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="V8" s="5">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5">
         <v>0.01</v>
       </c>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" dyDescent="0.25">
-      <c r="A10">
-        <v>80</v>
-      </c>
-      <c r="B10">
-        <v>35</v>
-      </c>
-      <c r="C10">
-        <v>0.02</v>
-      </c>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5">
+        <v>29.5</v>
+      </c>
+      <c r="G9" s="5">
+        <v>93.5</v>
+      </c>
+      <c r="H9" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="J9" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K9" s="5">
+        <v>42</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="5">
+        <v>50</v>
+      </c>
+      <c r="O9" s="5">
+        <v>25</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>29.5</v>
+      </c>
+      <c r="R9" s="5">
+        <v>93.5</v>
+      </c>
+      <c r="S9" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="T9" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="U9" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V9" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
+  <mergeCells count="3">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>